<commit_message>
Tile template and CSV exporting support
Finalized the board creation template. Added scripts for quickly
exporting multiple csvs from an excel file.
</commit_message>
<xml_diff>
--- a/tileTemplate.xlsx
+++ b/tileTemplate.xlsx
@@ -5,18 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy Jones\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neumont\RichAnimation\RichAnimationFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="BoardGraphics" sheetId="6" r:id="rId1"/>
+    <sheet name="BoardContents" sheetId="3" r:id="rId2"/>
+    <sheet name="BoardTriggers" sheetId="4" r:id="rId3"/>
+    <sheet name="BoardEnums" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="TileTypes">Sheet2!$A$1:$A$4</definedName>
+    <definedName name="contentEnums">BoardEnums!$B$2:$B$35</definedName>
+    <definedName name="graphicEnums">BoardEnums!$A$2:$A$36</definedName>
+    <definedName name="triggerEnums">BoardEnums!$C$2:$C$29</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>forestGrass</t>
   </si>
@@ -40,6 +44,30 @@
   </si>
   <si>
     <t>forestDirt</t>
+  </si>
+  <si>
+    <t>Graphic Enums</t>
+  </si>
+  <si>
+    <t>Content Enums</t>
+  </si>
+  <si>
+    <t>Trigger Enums</t>
+  </si>
+  <si>
+    <t>healthPotion</t>
+  </si>
+  <si>
+    <t>comfortSheep</t>
+  </si>
+  <si>
+    <t>bearTrap</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>jjss</t>
   </si>
 </sst>
 </file>
@@ -90,10 +118,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,19 +401,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -403,10 +427,8 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="2"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -423,10 +445,8 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="2"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -443,10 +463,8 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -463,10 +481,8 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -483,10 +499,8 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -503,10 +517,8 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -523,10 +535,8 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="2"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -543,10 +553,8 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="2"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -563,10 +571,8 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="2"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -583,10 +589,8 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="2"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -603,13 +607,11 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:Q11">
-      <formula1>TileTypes</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:P11">
+      <formula1>graphicEnums</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -618,34 +620,503 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:A4"/>
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:P11">
+      <formula1>contentEnums</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:P11">
+      <formula1>triggerEnums</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>